<commit_message>
test(api): more integ tests on valid files
</commit_message>
<xml_diff>
--- a/packages/api/tests/interfaces/http/fixtures/fixture.xlsx
+++ b/packages/api/tests/interfaces/http/fixtures/fixture.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t xml:space="preserve">random stuff</t>
   </si>
@@ -83,61 +83,31 @@
     <t xml:space="preserve">Ville d'Antibes</t>
   </si>
   <si>
-    <t xml:space="preserve">Convention délibération N° 1323-21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEA DU PERSONNEL DE LA VILLE D'ANTIBES JUAN-LES-PINS</t>
+    <t xml:space="preserve">Convention délibération N° 29-21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSOCIATION SPORTIVE AUTOMOBILE D'ANTIBES JUAN-LES-PINS</t>
   </si>
   <si>
     <t xml:space="preserve">fonctionnement</t>
   </si>
   <si>
-    <t xml:space="preserve">97176.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-03;2024-05-27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-03/2024-05-27</t>
+    <t xml:space="preserve">2024-01-25;2024-03-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-25/2024-03-29</t>
   </si>
   <si>
     <t xml:space="preserve">non</t>
   </si>
   <si>
+    <t xml:space="preserve">Convention délibération N° 2706-22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSOCIATION SPORTIVE DE LA FONTONNE-FOOTBALL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Convention délibération N° 3086-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTIBES RALLYE ASSOCIATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonjour toto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 2024-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTIBES BRIDGE ET JEUX DE L'ESPRIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pas un rna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 29-21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASSOCIATION SPORTIVE AUTOMOBILE D'ANTIBES JUAN-LES-PINS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-01-25;2024-03-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-01-25/2024-03-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 2706-22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASSOCIATION SPORTIVE DE LA FONTONNE-FOOTBALL</t>
   </si>
   <si>
     <t xml:space="preserve">AS FONTONNE ANTIBES-HOCKEY </t>
@@ -156,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -215,12 +186,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,322 +345,208 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>44352</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>45473</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="G4" s="1" t="n">
+        <v>38033590100027</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="n">
+        <v>135000</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>44530</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>45900</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="2" t="n">
+        <v>44834</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>46203</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>41925390100013</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="G5" s="1" t="n">
+        <v>37939422400016</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="0" t="n">
-        <v>33000</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>26</v>
+      <c r="K5" s="1" t="n">
+        <v>125000</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>45446</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>45446</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>92391758700019</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="C6" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>42901366700028</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>75000</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>45393</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>45393</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>44229</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>45473</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>38033590100027</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>135000</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>44834</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>46203</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>37939422400016</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>125000</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>44530</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>45900</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>42901366700028</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>90000</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="L6" s="2" t="n">
         <v>45380</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="M6" s="2" t="n">
         <v>45380</v>
       </c>
-      <c r="O9" s="0" t="s">
-        <v>26</v>
+      <c r="O6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: #3149 extract call to parsing from interface to service (#3230)
* test(api): more integ tests on valid files

* refactor(api): extract call to parser in service

* test(api): test boilerplate service function
</commit_message>
<xml_diff>
--- a/packages/api/tests/interfaces/http/fixtures/fixture.xlsx
+++ b/packages/api/tests/interfaces/http/fixtures/fixture.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t xml:space="preserve">random stuff</t>
   </si>
@@ -83,61 +83,31 @@
     <t xml:space="preserve">Ville d'Antibes</t>
   </si>
   <si>
-    <t xml:space="preserve">Convention délibération N° 1323-21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEA DU PERSONNEL DE LA VILLE D'ANTIBES JUAN-LES-PINS</t>
+    <t xml:space="preserve">Convention délibération N° 29-21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSOCIATION SPORTIVE AUTOMOBILE D'ANTIBES JUAN-LES-PINS</t>
   </si>
   <si>
     <t xml:space="preserve">fonctionnement</t>
   </si>
   <si>
-    <t xml:space="preserve">97176.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-03;2024-05-27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-03/2024-05-27</t>
+    <t xml:space="preserve">2024-01-25;2024-03-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-25/2024-03-29</t>
   </si>
   <si>
     <t xml:space="preserve">non</t>
   </si>
   <si>
+    <t xml:space="preserve">Convention délibération N° 2706-22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSOCIATION SPORTIVE DE LA FONTONNE-FOOTBALL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Convention délibération N° 3086-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTIBES RALLYE ASSOCIATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonjour toto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 2024-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANTIBES BRIDGE ET JEUX DE L'ESPRIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pas un rna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 29-21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASSOCIATION SPORTIVE AUTOMOBILE D'ANTIBES JUAN-LES-PINS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-01-25;2024-03-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-01-25/2024-03-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convention délibération N° 2706-22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASSOCIATION SPORTIVE DE LA FONTONNE-FOOTBALL</t>
   </si>
   <si>
     <t xml:space="preserve">AS FONTONNE ANTIBES-HOCKEY </t>
@@ -156,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -215,12 +186,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,322 +345,208 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>44352</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>45473</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="G4" s="1" t="n">
+        <v>38033590100027</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="n">
+        <v>135000</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>44530</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>45900</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="2" t="n">
+        <v>44834</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>46203</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>41925390100013</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="G5" s="1" t="n">
+        <v>37939422400016</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="0" t="n">
-        <v>33000</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>26</v>
+      <c r="K5" s="1" t="n">
+        <v>125000</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>21060004500012</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>45446</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>45446</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>92391758700019</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="C6" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>42901366700028</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>75000</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>45393</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>45393</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>44229</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>45473</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>38033590100027</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>135000</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>44834</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>46203</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>37939422400016</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>125000</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>21060004500012</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>44530</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>45900</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>42901366700028</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>90000</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="L6" s="2" t="n">
         <v>45380</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="M6" s="2" t="n">
         <v>45380</v>
       </c>
-      <c r="O9" s="0" t="s">
-        <v>26</v>
+      <c r="O6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>